<commit_message>
werite to file ready for testing
</commit_message>
<xml_diff>
--- a/rock_properties.xlsx
+++ b/rock_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!Work\Projects\mm_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865257A6-4D17-415F-8012-394AF040DF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C17959B-8A6D-4401-8667-1391378C828E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32010" yWindow="420" windowWidth="22590" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31530" yWindow="1410" windowWidth="22590" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet 1" sheetId="1" r:id="rId1"/>
@@ -204,10 +204,10 @@
     <t>Meta_Carb</t>
   </si>
   <si>
-    <t>Pyxenite_Hbnd</t>
-  </si>
-  <si>
     <t>Amphib</t>
+  </si>
+  <si>
+    <t>Pyxen_Hbnd</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>

</xml_diff>